<commit_message>
Implementação de envio de email na abertura e finalização
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28910"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\tickets_entrega\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FB0048D-6A1D-4A9C-A6C3-00542C09550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16403CC-3396-43B9-803B-FE2C1838B987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{52E17E58-EB7C-41A6-A909-4B7E1F6FB134}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="97">
   <si>
     <t>Cliente</t>
   </si>
@@ -179,13 +179,145 @@
   </si>
   <si>
     <t>XAVIER E AMORIM TRANSPORTES</t>
+  </si>
+  <si>
+    <t>enviar_para_email</t>
+  </si>
+  <si>
+    <t>email_copia</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>logistica4@aureaalimentos.com.br</t>
+  </si>
+  <si>
+    <t>sac2@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>atendimento2@aguiaramorim.com.br</t>
+  </si>
+  <si>
+    <t>;suporte@aguiaramorim.com.br;sac2@aguiaramorim.com.br;pendencia@aguiaramorim.com.br;sac3@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>vendas@baly.com.br</t>
+  </si>
+  <si>
+    <t>focal@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>ana.pires@jureiaalimentos.com.br</t>
+  </si>
+  <si>
+    <t>sac1@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>logistica@bilu.com.br</t>
+  </si>
+  <si>
+    <t>biri@biri.ind.br</t>
+  </si>
+  <si>
+    <t>sac@transfeliz.com.br</t>
+  </si>
+  <si>
+    <t>henrique@transfeliz.com.br;carolina@transfeliz.com.br;sac3@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>monitoramento@embrast.com.br</t>
+  </si>
+  <si>
+    <t>renato.rythowen@eolog.com</t>
+  </si>
+  <si>
+    <t>marcos.aurelio@eolog.com.br;sac3@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>ocorrencias@kisabor.ind.br</t>
+  </si>
+  <si>
+    <t>manoel@guimaraespl.com.br</t>
+  </si>
+  <si>
+    <t>leticia.flores@zeze.com.br</t>
+  </si>
+  <si>
+    <t>atendimento6@logdi.com.br</t>
+  </si>
+  <si>
+    <t>sac@mettabrasillogistica.com.br</t>
+  </si>
+  <si>
+    <t>;trafego@mettabrasillogistica.com.br;rastreamento@mettabrasillogistica.com.br;sac3@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>crm@moinhodonordeste.com.br</t>
+  </si>
+  <si>
+    <t>luciano.lopes@moinhodonordeste.com.br;sac2@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>saclogistica@tondo.com.br</t>
+  </si>
+  <si>
+    <t>lidiane.wagner@orquidea.com.br;sac2@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>alihezer.silva@mrcook.com.br</t>
+  </si>
+  <si>
+    <t>mauriciogoncalves.jms@hotmail.com;sac2@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>glauco.fleuri@novofrescor.com.br</t>
+  </si>
+  <si>
+    <t>selmipoa@selmi.com.br</t>
+  </si>
+  <si>
+    <t>posvendas1@plasutil.com.br</t>
+  </si>
+  <si>
+    <t>adriana.tonoli@plasvale.com.br</t>
+  </si>
+  <si>
+    <t>susi.oliveira@ponzan.com.br</t>
+  </si>
+  <si>
+    <t>seven@naga.com.br</t>
+  </si>
+  <si>
+    <t>operacional.poa@todobrasil.log.br</t>
+  </si>
+  <si>
+    <t>gerencia.poa@todobrasil.log.br;sac2@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sac6.sp@tjbtransportes.com.br </t>
+  </si>
+  <si>
+    <t>sac.rj@tjbtransportes.com.br;sac.poa@tjbtransportes.com.br;sac3@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>rodrigo@clicklogtransportes.com.br;paulo@clicklogtransportes.com.br</t>
+  </si>
+  <si>
+    <t>eurafaelmedeiros@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +452,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -618,7 +758,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -661,11 +801,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -695,6 +843,7 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hiperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
@@ -709,7 +858,26 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -720,6 +888,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D1A6003-AD6B-420F-B8FD-891612A2B579}" name="Tabela2" displayName="Tabela2" ref="A1:D45" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D45" xr:uid="{0D1A6003-AD6B-420F-B8FD-891612A2B579}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D44">
+    <sortCondition ref="A1:A44"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8DC57E86-0FB3-40B3-BDF2-C3CA9F749020}" name="Cliente" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4D394474-7295-4331-9D02-483D65F93D48}" name="Focal" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3A76E7B0-BC81-41A6-96D0-F9FE0FB05164}" name="enviar_para_email" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2E395DEA-50F0-4B9C-B816-5D60148E5CC5}" name="email_copia" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1039,365 +1223,654 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76EBC0C-1615-4DFC-BD6E-22E70D5FB3B8}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C37" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{D9003C5C-3976-4A85-84F9-9B237DD2F850}"/>
+    <hyperlink ref="C38" r:id="rId2" xr:uid="{D48B5608-77E8-4655-B5DC-33A18BD1112D}"/>
+    <hyperlink ref="C37" r:id="rId3" xr:uid="{F7DADD4D-52AC-45C3-B72C-6BA80BEFDBF5}"/>
+    <hyperlink ref="C36" r:id="rId4" xr:uid="{976065DB-E912-4BC6-90E8-7DE9A870855B}"/>
+    <hyperlink ref="C35" r:id="rId5" xr:uid="{FAF31D9C-BAAD-4026-AF42-A374AAB19B27}"/>
+    <hyperlink ref="C24" r:id="rId6" xr:uid="{0F0E793E-D3E0-4501-92AA-0FBE0ACA9582}"/>
+    <hyperlink ref="C23" r:id="rId7" xr:uid="{C4A916CE-E516-463B-9CC9-9E1417330B2C}"/>
+    <hyperlink ref="C22" r:id="rId8" xr:uid="{2FF926B0-9E5B-43BE-8215-37A1B7538235}"/>
+    <hyperlink ref="C18" r:id="rId9" xr:uid="{D4E79195-E761-4206-AE05-FB85E48B886F}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{50DB6CC9-A8ED-488E-95E8-A8C016D2DEEF}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{8C70D519-E5C6-4DB6-B04E-24A429A455E6}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{EEE992FD-9460-458C-9A17-BA90502683BC}"/>
+    <hyperlink ref="C21" r:id="rId13" xr:uid="{056E78F0-5BA0-45A9-A268-ADCAFA6EA41F}"/>
+    <hyperlink ref="C34" r:id="rId14" xr:uid="{22C516E5-3522-45BE-828E-C5F67E908608}"/>
+    <hyperlink ref="C6" r:id="rId15" xr:uid="{443B64A5-35EF-49EF-969A-F6923542F77D}"/>
+    <hyperlink ref="C12" r:id="rId16" xr:uid="{1164D05E-041D-4217-8522-AF445ADB09A8}"/>
+    <hyperlink ref="C20" r:id="rId17" xr:uid="{890ACA54-A4DD-472D-A6EE-EA4482B06391}"/>
+    <hyperlink ref="C28" r:id="rId18" xr:uid="{D7101A34-D1A3-4576-9715-A05F201ED4A8}"/>
+    <hyperlink ref="D28" r:id="rId19" xr:uid="{23320200-0AE3-4806-AE7D-DDE9471D6290}"/>
+    <hyperlink ref="C29" r:id="rId20" xr:uid="{29F7C5FB-B2C6-4E00-90CE-525A2A52EDE7}"/>
+    <hyperlink ref="D29" r:id="rId21" xr:uid="{A255BF9E-0F74-4763-8072-A35F58A421D3}"/>
+    <hyperlink ref="C40" r:id="rId22" xr:uid="{C1500DF4-96DA-4ED7-B5AB-D464962FC05C}"/>
+    <hyperlink ref="D40" r:id="rId23" xr:uid="{B6B748D9-B355-4616-9896-661673A87DBD}"/>
+    <hyperlink ref="C41" r:id="rId24" xr:uid="{7A695E45-2E79-41FD-B3AE-3A78288E0DC0}"/>
+    <hyperlink ref="D41" r:id="rId25" xr:uid="{FD7326B4-77F0-4BF6-BF28-562E394B257B}"/>
+    <hyperlink ref="C30" r:id="rId26" xr:uid="{D66CB11B-C3E4-4678-B457-E4BCE976FC62}"/>
+    <hyperlink ref="D30" r:id="rId27" xr:uid="{734E64F0-D062-4D4A-A517-287ADF2A867B}"/>
+    <hyperlink ref="C33" r:id="rId28" xr:uid="{F579E60C-F1F2-4554-B547-9286B7F2B3EF}"/>
+    <hyperlink ref="C7" r:id="rId29" xr:uid="{50748FF0-CD13-496A-B740-EFDCD7C21667}"/>
+    <hyperlink ref="C13" r:id="rId30" xr:uid="{227F93B3-255B-46D6-AF4E-63A6FCA82B36}"/>
+    <hyperlink ref="C14" r:id="rId31" xr:uid="{6B2D872C-DD3D-4966-A510-2E0C0BACE286}"/>
+    <hyperlink ref="C19" r:id="rId32" xr:uid="{B7C0B1B5-7D60-46C7-BB4E-8F7A768593D0}"/>
+    <hyperlink ref="C26" r:id="rId33" xr:uid="{6805F0C2-147C-4CD1-A4FC-6775B1D94F1B}"/>
+    <hyperlink ref="C27" r:id="rId34" xr:uid="{C18472B2-6AF0-49D3-9429-576E9366C004}"/>
+    <hyperlink ref="D19" r:id="rId35" xr:uid="{FBF0CF62-8321-48C7-98A0-DF47918A71B3}"/>
+    <hyperlink ref="C43" r:id="rId36" xr:uid="{51B18494-45AA-4DB2-9536-B6FDE6D9ADB0}"/>
+    <hyperlink ref="C44" r:id="rId37" xr:uid="{048ADA5B-05B1-453F-9912-7B7D23218E3D}"/>
+    <hyperlink ref="D13" r:id="rId38" xr:uid="{8683A207-A70F-4C9F-AE2A-2B318546B7EF}"/>
+    <hyperlink ref="D14" r:id="rId39" xr:uid="{84583E90-903B-4E5C-A55D-9372A24E34AA}"/>
+    <hyperlink ref="D43" r:id="rId40" xr:uid="{BBF1962D-68BB-4E98-B4A0-579D33DE5E53}"/>
+    <hyperlink ref="D18" r:id="rId41" display="biri@biri.ind.br" xr:uid="{ACCA0632-2092-4676-91B4-E4D5E5D00113}"/>
+    <hyperlink ref="D9:D12" r:id="rId42" display="biri@biri.ind.br" xr:uid="{A5222699-7918-44C3-A7B6-8C4DAE6DCD56}"/>
+    <hyperlink ref="D45" r:id="rId43" xr:uid="{DCBE0475-9B46-472A-8E91-D86C88ED948A}"/>
+    <hyperlink ref="C45" r:id="rId44" xr:uid="{81E2970F-6E36-46FF-9AA3-C72ABB168012}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId45"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>